<commit_message>
update task assign and deadlines
</commit_message>
<xml_diff>
--- a/Requirements/Travelling Social Network - File Tham Dinh Excel.xlsx
+++ b/Requirements/Travelling Social Network - File Tham Dinh Excel.xlsx
@@ -14,13 +14,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="128">
   <si>
     <t>STT</t>
   </si>
@@ -384,6 +385,30 @@
   </si>
   <si>
     <t>Functional Requirements</t>
+  </si>
+  <si>
+    <t>Trung</t>
+  </si>
+  <si>
+    <t>Nhan</t>
+  </si>
+  <si>
+    <t>Thang</t>
+  </si>
+  <si>
+    <t>Hung</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>6/4/2014 12:00AM</t>
+  </si>
+  <si>
+    <t>8/4/2013 12:00AM</t>
   </si>
 </sst>
 </file>
@@ -433,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,6 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1261,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,280 +1298,598 @@
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>119</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>73</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="D15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>78</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="D21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>84</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>91</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>121</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="D34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>96</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="D36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="D37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="D38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="D39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>51</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="D43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>52</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+      <c r="D46" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="D47" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>118</v>
       </c>
+      <c r="D48" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "update task assign and deadlines"
This reverts commit e79a942b82a26a48304ee85346c0aeb784f79922.
</commit_message>
<xml_diff>
--- a/Requirements/Travelling Social Network - File Tham Dinh Excel.xlsx
+++ b/Requirements/Travelling Social Network - File Tham Dinh Excel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="128">
   <si>
     <t>STT</t>
   </si>
@@ -408,10 +408,7 @@
     <t>6/4/2014 12:00AM</t>
   </si>
   <si>
-    <t>6/4/2013 12:00AM</t>
-  </si>
-  <si>
-    <t>6/6/2013 12:00AM</t>
+    <t>8/4/2013 12:00AM</t>
   </si>
 </sst>
 </file>
@@ -1292,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:E48"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1569,7 @@
         <v>121</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1583,7 +1580,7 @@
         <v>121</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -1597,7 +1594,7 @@
         <v>121</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1608,7 +1605,7 @@
         <v>121</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -1619,7 +1616,7 @@
         <v>121</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1630,7 +1627,7 @@
         <v>121</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -1641,7 +1638,7 @@
         <v>121</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -1652,7 +1649,7 @@
         <v>121</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1666,7 +1663,7 @@
         <v>121</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -1677,7 +1674,7 @@
         <v>121</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -1688,7 +1685,7 @@
         <v>121</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -1699,7 +1696,7 @@
         <v>121</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -1713,7 +1710,7 @@
         <v>122</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -1724,7 +1721,7 @@
         <v>122</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -1735,7 +1732,7 @@
         <v>120</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1746,7 +1743,7 @@
         <v>120</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -1757,7 +1754,7 @@
         <v>120</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -1771,7 +1768,7 @@
         <v>123</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -1782,7 +1779,7 @@
         <v>123</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -1793,7 +1790,7 @@
         <v>123</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -1804,7 +1801,7 @@
         <v>123</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
@@ -1818,7 +1815,7 @@
         <v>123</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
@@ -1829,7 +1826,7 @@
         <v>123</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
@@ -1840,7 +1837,7 @@
         <v>123</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -1851,7 +1848,7 @@
         <v>123</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -1862,7 +1859,7 @@
         <v>122</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>